<commit_message>
Minor fixes in executable files and added results for MapRDB benches
</commit_message>
<xml_diff>
--- a/bench times_xml.xlsx
+++ b/bench times_xml.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t xml:space="preserve">master</t>
   </si>
@@ -65,7 +65,23 @@
     <t xml:space="preserve">15mins, 24sec</t>
   </si>
   <si>
+    <t xml:space="preserve">Maprdb-scan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hibench.join.bigdata.uservisits                 5000000000
+hibench.join.bigdata.pages                      120000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15mins, 25sec</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maprdb-join</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24mins, 45sec</t>
   </si>
 </sst>
 </file>
@@ -239,21 +255,22 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4540816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.219387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.8877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.2040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.9642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.75"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.5765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9795918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3520408163265"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.86734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -320,7 +337,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="49.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
@@ -334,22 +351,22 @@
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>5</v>
+      <c r="H3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -366,10 +383,22 @@
         <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change _id field generator, added path for MapRDB
</commit_message>
<xml_diff>
--- a/bench times_xml.xlsx
+++ b/bench times_xml.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t xml:space="preserve">master</t>
   </si>
@@ -62,23 +63,27 @@
 Hibench.aggregation.bigdata.pages 500000000</t>
   </si>
   <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
     <t xml:space="preserve">15mins, 24sec</t>
   </si>
   <si>
     <t xml:space="preserve">Maprdb-scan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hibench.join.bigdata.uservisits                 2000000000
+hibench.join.bigdata.pages                      120000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15mins, 25sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maprdb-join</t>
   </si>
   <si>
     <t xml:space="preserve">hibench.join.bigdata.uservisits                 5000000000
 hibench.join.bigdata.pages                      120000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15mins, 25sec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maprdb-join</t>
   </si>
   <si>
     <t xml:space="preserve">24mins, 45sec</t>
@@ -255,22 +260,22 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.9642857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.75"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.5765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9795918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3520408163265"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.86734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.9795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4285714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.2142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -327,17 +332,17 @@
       <c r="G2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>90</v>
+      <c r="H2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="49.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
@@ -351,19 +356,19 @@
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>17</v>
@@ -386,19 +391,19 @@
         <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -410,4 +415,30 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>